<commit_message>
Dodałem funkcję celu oraz ograniczenia
</commit_message>
<xml_diff>
--- a/MMO.xlsx
+++ b/MMO.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Arkusz2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Arkusz3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t xml:space="preserve">Produkt</t>
   </si>
@@ -45,6 +45,9 @@
     <t xml:space="preserve">Pojemność Bagażnika w litrach</t>
   </si>
   <si>
+    <t xml:space="preserve">Tablica Rejestracyjna</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oznaczenia</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
     <t xml:space="preserve">Japoński</t>
   </si>
   <si>
+    <t xml:space="preserve">TTR55OP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volkswagen Polo</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
     <t xml:space="preserve">Niemiecki</t>
   </si>
   <si>
+    <t xml:space="preserve">ELW930TR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Honda Civic</t>
   </si>
   <si>
@@ -126,6 +135,9 @@
     <t xml:space="preserve">Amerykański</t>
   </si>
   <si>
+    <t xml:space="preserve">WR095TT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ford Mondeo</t>
   </si>
   <si>
@@ -141,6 +153,9 @@
     <t xml:space="preserve">Brytyjski</t>
   </si>
   <si>
+    <t xml:space="preserve">EL123KC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cadillac STS</t>
   </si>
   <si>
@@ -156,6 +171,9 @@
     <t xml:space="preserve">Włoski</t>
   </si>
   <si>
+    <t xml:space="preserve">EL187CP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jaguar XJ</t>
   </si>
   <si>
@@ -171,6 +189,9 @@
     <t xml:space="preserve">Francuski</t>
   </si>
   <si>
+    <t xml:space="preserve">KRT950PP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ferrari 458 Italia</t>
   </si>
   <si>
@@ -183,6 +204,9 @@
     <t xml:space="preserve">Koreański</t>
   </si>
   <si>
+    <t xml:space="preserve">354P545</t>
+  </si>
+  <si>
     <t xml:space="preserve">Audi Q7</t>
   </si>
   <si>
@@ -195,6 +219,9 @@
     <t xml:space="preserve">Czeski</t>
   </si>
   <si>
+    <t xml:space="preserve">TR906PP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volkswagen Transporter</t>
   </si>
   <si>
@@ -219,6 +246,9 @@
     <t xml:space="preserve">Indyjski</t>
   </si>
   <si>
+    <t xml:space="preserve">5045T05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Citroen C1</t>
   </si>
   <si>
@@ -228,6 +258,9 @@
     <t xml:space="preserve">Hiszpański</t>
   </si>
   <si>
+    <t xml:space="preserve">PIO402LL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hyundai i20</t>
   </si>
   <si>
@@ -237,118 +270,235 @@
     <t xml:space="preserve">Rosyjski</t>
   </si>
   <si>
+    <t xml:space="preserve">LL04040T</t>
+  </si>
+  <si>
     <t xml:space="preserve">Skoda Oktavia</t>
   </si>
   <si>
+    <t xml:space="preserve">TTT34LWR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volvo S40</t>
   </si>
   <si>
+    <t xml:space="preserve">UJR90900</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lexus GS</t>
   </si>
   <si>
+    <t xml:space="preserve">90904TTTT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rolls-Royce Phantom</t>
   </si>
   <si>
+    <t xml:space="preserve">TR30RT30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercedes-Benz SLS AMG</t>
   </si>
   <si>
+    <t xml:space="preserve">WRT3209T</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mitsubishi Outlander</t>
   </si>
   <si>
+    <t xml:space="preserve">KW0988T</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chrysler Voyager</t>
   </si>
   <si>
+    <t xml:space="preserve">WWW560TT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Opel Astra</t>
   </si>
   <si>
+    <t xml:space="preserve">GR9090HH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tata Nano</t>
   </si>
   <si>
+    <t xml:space="preserve">HWLR509K</t>
+  </si>
+  <si>
     <t xml:space="preserve">Skoda Fabia</t>
   </si>
   <si>
+    <t xml:space="preserve">KTR0909Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peugout 308</t>
   </si>
   <si>
+    <t xml:space="preserve">YUF509690</t>
+  </si>
+  <si>
     <t xml:space="preserve">Skoda Suberp</t>
   </si>
   <si>
+    <t xml:space="preserve">OP400UHK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercedes-Benz Klasy E</t>
   </si>
   <si>
+    <t xml:space="preserve">KML0903L</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercedes-Benz Klasy S</t>
   </si>
   <si>
+    <t xml:space="preserve">LWA989M</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nissan GT-R</t>
   </si>
   <si>
+    <t xml:space="preserve">MMW98TF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toyota Hilux</t>
   </si>
   <si>
+    <t xml:space="preserve">954FF342</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mercedes-Benz Viano</t>
   </si>
   <si>
+    <t xml:space="preserve">II540OP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aston Martin DB9 Volante</t>
   </si>
   <si>
+    <t xml:space="preserve">OPWT8909</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kia Picanto</t>
   </si>
   <si>
+    <t xml:space="preserve">9090TI59</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fiat Punto</t>
   </si>
   <si>
+    <t xml:space="preserve">GH4958TT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volkswagen Golf</t>
   </si>
   <si>
+    <t xml:space="preserve">GOP909UU</t>
+  </si>
+  <si>
     <t xml:space="preserve">BMW M3</t>
   </si>
   <si>
+    <t xml:space="preserve">UH493KW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toyota Prius</t>
   </si>
   <si>
+    <t xml:space="preserve">WN890IJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lincoln Town Car</t>
   </si>
   <si>
+    <t xml:space="preserve">IWO000OO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bugatti Veyron</t>
   </si>
   <si>
+    <t xml:space="preserve">FR404UU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dodge RAM</t>
   </si>
   <si>
+    <t xml:space="preserve">ERR1010B</t>
+  </si>
+  <si>
     <t xml:space="preserve">GMC Safari</t>
   </si>
   <si>
+    <t xml:space="preserve">BRT04000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lexus IS</t>
   </si>
   <si>
+    <t xml:space="preserve">TRA90905</t>
+  </si>
+  <si>
     <t xml:space="preserve">Smart</t>
   </si>
   <si>
+    <t xml:space="preserve">5903IIT4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seat Ibiza</t>
   </si>
   <si>
+    <t xml:space="preserve">LA953NBM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lada Priora</t>
   </si>
   <si>
+    <t xml:space="preserve">URI054LL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nissan Primera</t>
   </si>
   <si>
+    <t xml:space="preserve">LG4895HH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Audi A6</t>
   </si>
   <si>
+    <t xml:space="preserve">QQ894LR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lexus LS</t>
   </si>
   <si>
+    <t xml:space="preserve">RE545KMU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Koenigsegg Agera R</t>
   </si>
   <si>
+    <t xml:space="preserve">UIB8940P</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ford F-150</t>
   </si>
   <si>
+    <t xml:space="preserve">PL989OO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Renault Traffic</t>
   </si>
   <si>
+    <t xml:space="preserve">VFB804ST</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mazda MX-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM543GG</t>
   </si>
 </sst>
 </file>
@@ -358,7 +508,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -381,16 +531,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -398,8 +671,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,8 +711,56 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,15 +769,99 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -450,36 +870,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="1.92712550607287"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="1.92712550607287"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="1.92712550607287"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="1.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="1.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="1.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="18.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,37 +927,44 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1" t="s">
+      <c r="R1" s="1"/>
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="1"/>
+      <c r="W1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>54</v>
@@ -554,46 +984,55 @@
       <c r="G2" s="0" t="n">
         <v>138</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="P2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="R2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>131</v>
@@ -613,46 +1052,55 @@
       <c r="G3" s="0" t="n">
         <v>270</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="0" t="n">
+      <c r="K3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="M3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="P3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="0" t="n">
+      <c r="O3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="R3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="0" t="n">
+      <c r="Q3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="0" t="n">
+      <c r="S3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>174</v>
@@ -672,40 +1120,49 @@
       <c r="G4" s="0" t="n">
         <v>370</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="0" t="n">
+      <c r="K4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="N4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="0" t="n">
+      <c r="M4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="0" t="n">
+      <c r="O4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="T4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="U4" s="0" t="n">
+      <c r="Q4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>200</v>
@@ -725,34 +1182,43 @@
       <c r="G5" s="0" t="n">
         <v>550</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="0" t="n">
+      <c r="K5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="P5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="0" t="n">
+      <c r="O5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="T5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" s="0" t="n">
+      <c r="Q5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>324</v>
@@ -772,34 +1238,43 @@
       <c r="G6" s="0" t="n">
         <v>464</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="0" t="n">
-        <v>5</v>
+      <c r="H6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>470</v>
@@ -819,34 +1294,43 @@
       <c r="G7" s="0" t="n">
         <v>550</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="N7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="0" t="n">
+      <c r="K7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="P7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q7" s="0" t="n">
+      <c r="O7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="T7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="U7" s="0" t="n">
+      <c r="Q7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>570</v>
@@ -866,28 +1350,37 @@
       <c r="G8" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="P8" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q8" s="0" t="n">
+      <c r="K8" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="T8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="U8" s="0" t="n">
+      <c r="Q8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>272</v>
@@ -907,28 +1400,37 @@
       <c r="G9" s="0" t="n">
         <v>775</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="P9" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" s="0" t="n">
+      <c r="K9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="T9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="U9" s="0" t="n">
+      <c r="Q9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>204</v>
@@ -948,28 +1450,37 @@
       <c r="G10" s="0" t="n">
         <v>405</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="P10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q10" s="0" t="n">
+      <c r="K10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="T10" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="U10" s="0" t="n">
+      <c r="Q10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="R10" s="0" t="n">
         <v>9</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>315</v>
@@ -989,28 +1500,37 @@
       <c r="G11" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="J11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="P11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q11" s="0" t="n">
+      <c r="K11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="T11" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="U11" s="0" t="n">
+      <c r="Q11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="R11" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -1030,22 +1550,31 @@
       <c r="G12" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="P12" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="T12" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="U12" s="0" t="n">
+      <c r="Q12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="R12" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>116</v>
@@ -1065,22 +1594,31 @@
       <c r="G13" s="0" t="n">
         <v>295</v>
       </c>
-      <c r="P13" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="T13" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="U13" s="0" t="n">
+      <c r="Q13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="R13" s="0" t="n">
         <v>12</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>200</v>
@@ -1100,10 +1638,19 @@
       <c r="G14" s="0" t="n">
         <v>560</v>
       </c>
+      <c r="H14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>200</v>
@@ -1123,10 +1670,19 @@
       <c r="G15" s="0" t="n">
         <v>404</v>
       </c>
+      <c r="H15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>345</v>
@@ -1146,10 +1702,19 @@
       <c r="G16" s="0" t="n">
         <v>510</v>
       </c>
+      <c r="H16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>460</v>
@@ -1169,10 +1734,19 @@
       <c r="G17" s="0" t="n">
         <v>590</v>
       </c>
+      <c r="H17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>570</v>
@@ -1192,10 +1766,19 @@
       <c r="G18" s="0" t="n">
         <v>176</v>
       </c>
+      <c r="H18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>220</v>
@@ -1215,10 +1798,19 @@
       <c r="G19" s="0" t="n">
         <v>541</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>163</v>
@@ -1238,10 +1830,19 @@
       <c r="G20" s="0" t="n">
         <v>550</v>
       </c>
+      <c r="H20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>110</v>
@@ -1261,10 +1862,19 @@
       <c r="G21" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="H21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>33</v>
@@ -1284,10 +1894,19 @@
       <c r="G22" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="H22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>54</v>
@@ -1307,10 +1926,19 @@
       <c r="G23" s="0" t="n">
         <v>330</v>
       </c>
+      <c r="H23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>120</v>
@@ -1330,10 +1958,19 @@
       <c r="G24" s="0" t="n">
         <v>348</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="W24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>220</v>
@@ -1353,10 +1990,19 @@
       <c r="G25" s="0" t="n">
         <v>565</v>
       </c>
+      <c r="H25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="W25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>299</v>
@@ -1376,10 +2022,19 @@
       <c r="G26" s="0" t="n">
         <v>540</v>
       </c>
+      <c r="H26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="W26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>585</v>
@@ -1399,10 +2054,19 @@
       <c r="G27" s="0" t="n">
         <v>510</v>
       </c>
+      <c r="H27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>575</v>
@@ -1422,10 +2086,19 @@
       <c r="G28" s="0" t="n">
         <v>255</v>
       </c>
+      <c r="H28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="W28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>174</v>
@@ -1445,10 +2118,19 @@
       <c r="G29" s="0" t="n">
         <v>650</v>
       </c>
+      <c r="H29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="W29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>190</v>
@@ -1468,10 +2150,19 @@
       <c r="G30" s="0" t="n">
         <v>490</v>
       </c>
+      <c r="H30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="W30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>477</v>
@@ -1491,10 +2182,19 @@
       <c r="G31" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="H31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="W31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="X31" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>85</v>
@@ -1514,10 +2214,19 @@
       <c r="G32" s="0" t="n">
         <v>157</v>
       </c>
+      <c r="H32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="W32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>76</v>
@@ -1537,10 +2246,19 @@
       <c r="G33" s="0" t="n">
         <v>275</v>
       </c>
+      <c r="H33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="W33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="X33" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>220</v>
@@ -1560,10 +2278,19 @@
       <c r="G34" s="0" t="n">
         <v>498</v>
       </c>
+      <c r="H34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="W34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>420</v>
@@ -1583,10 +2310,19 @@
       <c r="G35" s="0" t="n">
         <v>550</v>
       </c>
+      <c r="H35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="W35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>98</v>
@@ -1606,10 +2342,19 @@
       <c r="G36" s="0" t="n">
         <v>445</v>
       </c>
+      <c r="H36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="W36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>239</v>
@@ -1629,10 +2374,19 @@
       <c r="G37" s="0" t="n">
         <v>540</v>
       </c>
+      <c r="H37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="W37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="X37" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1001</v>
@@ -1652,10 +2406,19 @@
       <c r="G38" s="0" t="n">
         <v>175</v>
       </c>
+      <c r="H38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="W38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>517</v>
@@ -1675,10 +2438,19 @@
       <c r="G39" s="0" t="n">
         <v>610</v>
       </c>
+      <c r="H39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>200</v>
@@ -1698,10 +2470,19 @@
       <c r="G40" s="0" t="n">
         <v>580</v>
       </c>
+      <c r="H40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>245</v>
@@ -1721,10 +2502,19 @@
       <c r="G41" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="H41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="X41" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>61</v>
@@ -1744,10 +2534,19 @@
       <c r="G42" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="H42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="W42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>105</v>
@@ -1767,10 +2566,19 @@
       <c r="G43" s="0" t="n">
         <v>267</v>
       </c>
+      <c r="H43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="W43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="X43" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>125</v>
@@ -1790,10 +2598,19 @@
       <c r="G44" s="0" t="n">
         <v>444</v>
       </c>
+      <c r="H44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="W44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>150</v>
@@ -1813,10 +2630,19 @@
       <c r="G45" s="0" t="n">
         <v>450</v>
       </c>
+      <c r="H45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="W45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>320</v>
@@ -1836,10 +2662,19 @@
       <c r="G46" s="0" t="n">
         <v>545</v>
       </c>
+      <c r="H46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="W46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>438</v>
@@ -1859,10 +2694,19 @@
       <c r="G47" s="0" t="n">
         <v>465</v>
       </c>
+      <c r="H47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="W47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="X47" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1140</v>
@@ -1882,10 +2726,19 @@
       <c r="G48" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="H48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="W48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>320</v>
@@ -1905,10 +2758,19 @@
       <c r="G49" s="0" t="n">
         <v>650</v>
       </c>
+      <c r="H49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="W49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="X49" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>115</v>
@@ -1928,10 +2790,19 @@
       <c r="G50" s="0" t="n">
         <v>480</v>
       </c>
+      <c r="H50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="W50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>165</v>
@@ -1951,15 +2822,25 @@
       <c r="G51" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="H51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="W51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="X51" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
+  <mergeCells count="7">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1978,13 +2859,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2004,13 +2885,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>